<commit_message>
Add 01 to 20 tricks
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Oliveira\Desktop\Documentos\Free Code Camp\free-code-camp\Front End Tricks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="HTML" sheetId="1" r:id="rId1"/>
-    <sheet name="CSS" sheetId="2" r:id="rId2"/>
+    <sheet name="Glossary" sheetId="6" r:id="rId1"/>
+    <sheet name="HTML-CSS" sheetId="1" r:id="rId2"/>
     <sheet name="Bootstrap" sheetId="3" r:id="rId3"/>
     <sheet name="Font Awesome" sheetId="4" r:id="rId4"/>
     <sheet name="Animated" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,28 +28,221 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Properties</t>
-  </si>
-  <si>
     <t>&lt;h1&gt; to &lt;h6&gt;</t>
   </si>
   <si>
-    <t>Heading 1 to 6</t>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_hn.asp </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_p.asp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_comment.asp </t>
+  </si>
+  <si>
+    <t>&lt;!--...--&gt;</t>
+  </si>
+  <si>
+    <t>The &lt;p&gt; tag defines a paragraph.</t>
+  </si>
+  <si>
+    <t>The comment tag is used to insert comments in the source code. Comments are not displayed in the browsers.</t>
+  </si>
+  <si>
+    <t>The &lt;h1&gt; to &lt;h6&gt; tags are used to define HTML headings.</t>
+  </si>
+  <si>
+    <t>Trick</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum</t>
+  </si>
+  <si>
+    <t>Placeholder Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://br.lipsum.com/ </t>
+  </si>
+  <si>
+    <t>Change color; Inline CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/html/html_styles.asp </t>
+  </si>
+  <si>
+    <t>&lt;tagname style="color: red"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;style&gt;</t>
+  </si>
+  <si>
+    <t>The &lt;style&gt; tag is used to define style information for an HTML document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_style.asp </t>
+  </si>
+  <si>
+    <t>&lt;tagname class="class-name"&gt;</t>
+  </si>
+  <si>
+    <t>The class attribute specifies one or more classnames for an element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_global_class.asp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/sel_class.asp </t>
+  </si>
+  <si>
+    <t>.class-name</t>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> selector selects elements with a specific class attribute.</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;tag&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tag attribute="value"&gt;</t>
+  </si>
+  <si>
+    <t>.selector</t>
+  </si>
+  <si>
+    <t>.selector {property;}</t>
+  </si>
+  <si>
+    <t>.class-name { font-size: 16px;}</t>
+  </si>
+  <si>
+    <t>The font-size property sets the size of a font.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_font_font-size.asp </t>
+  </si>
+  <si>
+    <t>The font-family property specifies the font for an element.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_font_font-family.asp </t>
+  </si>
+  <si>
+    <t>&lt;link&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_link.asp </t>
+  </si>
+  <si>
+    <t>The &lt;link&gt; tag defines a link between a document and an external resource.</t>
+  </si>
+  <si>
+    <t>Google Fonts</t>
+  </si>
+  <si>
+    <t>&lt;link href="https://fonts.googleapis.com/css?family={{font-family}}" rel="stylesheet" type="text/css"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fonts.google.com/ </t>
+  </si>
+  <si>
+    <t>.class-name { font-family: Helvetica, Monospace;}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_img.asp </t>
+  </si>
+  <si>
+    <t>&lt;img src="URL" alt="alternate text&gt;</t>
+  </si>
+  <si>
+    <t>The &lt;img&gt; tag defines an image in an HTML page.</t>
+  </si>
+  <si>
+    <t>.class-name { width: 100px;}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_dim_width.asp </t>
+  </si>
+  <si>
+    <t>The width property sets the width of an element.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_border-color.asp </t>
+  </si>
+  <si>
+    <t>The border-color property sets the color of an element's four borders. This property can have from one to four values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_border-width.asp </t>
+  </si>
+  <si>
+    <t>The border-width property sets the width of an element's four borders. This property can have from one to four values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_border-style.asp </t>
+  </si>
+  <si>
+    <t>The border-style property sets the style of an element's four borders. This property can have from one to four values.</t>
+  </si>
+  <si>
+    <t>.class-name {border-style: solid;}</t>
+  </si>
+  <si>
+    <t>.class-name {border-width: 10px;}</t>
+  </si>
+  <si>
+    <t>.class-name {border-color: green;}</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/cssref/css3_pr_border-radius.asp</t>
+  </si>
+  <si>
+    <t>The border-radius property is used to add rounded corners to an element.</t>
+  </si>
+  <si>
+    <t>.class-name {border-radius: 50%;}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +266,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -86,7 +301,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -96,26 +311,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+  <cellStyles count="10">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,56 +678,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D3"/>
+  <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="32" customHeight="1">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="2"/>
+    <col min="2" max="2" width="33.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId12"/>
+    <hyperlink ref="D15" r:id="rId13"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D17" r:id="rId15"/>
+    <hyperlink ref="D18" r:id="rId16"/>
+    <hyperlink ref="D19" r:id="rId17"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -503,9 +977,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -520,9 +994,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -537,9 +1011,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Add Tricks from Lessons 21 to 40
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
   <si>
     <t>Description</t>
   </si>
@@ -237,12 +237,221 @@
   <si>
     <t>.class-name {border-radius: 50%;}</t>
   </si>
+  <si>
+    <t>&lt;a href="URL"&gt;</t>
+  </si>
+  <si>
+    <t>The &lt;a&gt; tag defines a hyperlink, which is used to link from one page to another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_a.asp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_a_target.asp </t>
+  </si>
+  <si>
+    <t>The target attribute specifies where to open the linked document.</t>
+  </si>
+  <si>
+    <t>&lt;a href="URL" target="_blank|_self|_parent|_top|framename"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="#"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.freecodecamp.org/challenges/make-dead-links-using-the-hash-symbol </t>
+  </si>
+  <si>
+    <t>Replace the value of your a element's href attribute with a #, also known as a hash symbol, to turn it into a dead link.</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt; &lt;li&gt;List Item&lt;/li&gt;&lt;ul&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_ul.asp </t>
+  </si>
+  <si>
+    <t>The &lt;ul&gt; tag defines an unordered (bulleted) list. Use the &lt;ul&gt; tag together with the &lt;li&gt; tag to create unordered lists.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt; &lt;li&gt;List Item&lt;/li&gt;&lt;ol&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The &lt;ol&gt; tag defines an ordered list. An ordered list can be numerical or alphabetical. Use the &lt;li&gt; tag to define list items.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_ol.asp </t>
+  </si>
+  <si>
+    <t>&lt;input type="text"&gt;</t>
+  </si>
+  <si>
+    <t>The &lt;input&gt; tag specifies an input field where the user can enter data. &lt;input&gt; elements are used within a &lt;form&gt; element to declare input controls that allow users to input data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_input.asp </t>
+  </si>
+  <si>
+    <t>&lt;input type="text" placeholder="Lorem Ipsum"&gt;</t>
+  </si>
+  <si>
+    <t>The placeholder attribute specifies a short hint that describes the expected value of an input field (e.g. a sample value or a short description of the expected format). The short hint is displayed in the input field before the user enters a value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_input_placeholder.asp </t>
+  </si>
+  <si>
+    <t>The &lt;form&gt; tag is used to create an HTML form for user input.</t>
+  </si>
+  <si>
+    <t>&lt;input&gt;</t>
+  </si>
+  <si>
+    <t>&lt;form&gt; &lt;input&gt;&lt;/form&gt;</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/att_input_type.asp</t>
+  </si>
+  <si>
+    <t>The type attribute specifies the type of &lt;input&gt; element to display. The default type is text.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_form.asp </t>
+  </si>
+  <si>
+    <t>The action attribute specifies where to send the form-data when a form is submitted.</t>
+  </si>
+  <si>
+    <t>&lt;form action="/submit-cat-photo"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_form_action.asp </t>
+  </si>
+  <si>
+    <t>&lt;button type="submit"&gt;Submit&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_button.asp </t>
+  </si>
+  <si>
+    <t>The &lt;button&gt; tag defines a clickable button. Inside a &lt;button&gt; element you can put content, like text or images. This is the difference between this element and buttons created with the &lt;input&gt; element.</t>
+  </si>
+  <si>
+    <t>&lt;button&gt;Submit&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_button_type.asp </t>
+  </si>
+  <si>
+    <t>The type attribute specifies the type of button.</t>
+  </si>
+  <si>
+    <t>&lt;input type="text" placeholder="cat photo URL" required&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_input_required.asp </t>
+  </si>
+  <si>
+    <t>The required attribute is a boolean attribute. When present, it specifies that an input field must be filled out before submitting the form.</t>
+  </si>
+  <si>
+    <t>&lt;label&gt;&lt;input type="radio" name="indoor-outdoor"&gt;Indoor&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;label&gt;&lt;input type="radio"&gt;Indoor&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;input type="radio"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_input_type.asp </t>
+  </si>
+  <si>
+    <t>&lt;input type="checkbox"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_label.asp </t>
+  </si>
+  <si>
+    <t>The &lt;label&gt; tag defines a label for an &lt;input&gt; element. The &lt;label&gt; element does not render as anything special for the user. However, it provides a usability improvement for mouse users, because if the user clicks on the text within the &lt;label&gt; element, it toggles the control.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_input_name.asp </t>
+  </si>
+  <si>
+    <t>The name attribute specifies the name of an &lt;input&gt; element. The name attribute is used to reference elements in a JavaScript, or to reference form data after a form is submitted.</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_div.asp </t>
+  </si>
+  <si>
+    <t>The &lt;div&gt; tag defines a division or a section in an HTML document. The &lt;div&gt; tag is used to group block-elements to format them with CSS.</t>
+  </si>
+  <si>
+    <t>&lt;div class="class-name"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .class-name {
+    background-color: value;
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_background-color.asp </t>
+  </si>
+  <si>
+    <t>The background-color property sets the background color of an element. The background of an element is the total size of the element, including padding and border (but not the margin).</t>
+  </si>
+  <si>
+    <t>&lt;element id="id-value"&gt;</t>
+  </si>
+  <si>
+    <t>The id attribute specifies a unique id for an HTML element (the value must be unique within the HTML document). The id attribute is most used to point to a style in a style sheet, and by JavaScript (via the HTML DOM) to manipulate the element with the specific id.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/att_global_id.asp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  #id-value {
+    property: value;
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/sel_id.asp </t>
+  </si>
+  <si>
+    <t>The #id selector styles the element with the specified id.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .selector {
+    padding: value;
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/css/css_padding.asp </t>
+  </si>
+  <si>
+    <t>The CSS padding properties are used to generate space around content. The padding clears an area around the content (inside the border) of an element.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .selector {
+    margin: value;
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/css/css_margin.asp </t>
+  </si>
+  <si>
+    <t>The CSS margin properties are used to generate space around elements. The margin properties set the size of the white space outside the border.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +492,13 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -313,7 +529,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,6 +544,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -716,22 +938,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D20"/>
+  <dimension ref="B2:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A43" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="92.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="33.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
@@ -742,7 +964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -753,7 +975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -764,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -775,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
@@ -786,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
@@ -797,7 +1019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -808,7 +1030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -819,7 +1041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
@@ -830,7 +1052,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
@@ -841,7 +1063,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
@@ -852,7 +1074,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
@@ -863,7 +1085,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
@@ -874,7 +1096,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -885,7 +1107,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
@@ -896,8 +1118,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -907,7 +1129,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
@@ -918,7 +1140,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
@@ -929,10 +1151,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>20</v>
-      </c>
+    <row r="20" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>60</v>
       </c>
@@ -942,6 +1161,531 @@
       <c r="D20" s="3" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="21" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="7"/>
+    </row>
+    <row r="64" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="7"/>
+    </row>
+    <row r="65" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="7"/>
+    </row>
+    <row r="67" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="7"/>
+    </row>
+    <row r="68" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="7"/>
+    </row>
+    <row r="70" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="7"/>
+    </row>
+    <row r="75" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="7"/>
+    </row>
+    <row r="76" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="7"/>
+    </row>
+    <row r="77" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="7"/>
+    </row>
+    <row r="79" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="7"/>
+    </row>
+    <row r="81" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="7"/>
+    </row>
+    <row r="82" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="7"/>
+    </row>
+    <row r="83" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="7"/>
+    </row>
+    <row r="84" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="7"/>
+    </row>
+    <row r="85" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="7"/>
+    </row>
+    <row r="86" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="7"/>
+    </row>
+    <row r="88" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="7"/>
+    </row>
+    <row r="89" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="7"/>
+    </row>
+    <row r="90" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C90" s="7"/>
+    </row>
+    <row r="91" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C91" s="7"/>
+    </row>
+    <row r="92" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C94" s="7"/>
+    </row>
+    <row r="95" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C95" s="7"/>
+    </row>
+    <row r="96" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="7"/>
+    </row>
+    <row r="97" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="7"/>
+    </row>
+    <row r="98" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C98" s="7"/>
+    </row>
+    <row r="99" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C99" s="7"/>
+    </row>
+    <row r="100" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="7"/>
+    </row>
+    <row r="101" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="7"/>
+    </row>
+    <row r="102" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="7"/>
+    </row>
+    <row r="103" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="7"/>
+    </row>
+    <row r="104" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="7"/>
+    </row>
+    <row r="105" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="7"/>
+    </row>
+    <row r="106" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C106" s="7"/>
+    </row>
+    <row r="107" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C107" s="7"/>
+    </row>
+    <row r="108" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C108" s="7"/>
+    </row>
+    <row r="109" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C109" s="7"/>
+    </row>
+    <row r="110" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C110" s="7"/>
+    </row>
+    <row r="111" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C111" s="7"/>
+    </row>
+    <row r="112" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C112" s="7"/>
+    </row>
+    <row r="113" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C113" s="7"/>
+    </row>
+    <row r="114" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C114" s="7"/>
+    </row>
+    <row r="115" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C115" s="7"/>
+    </row>
+    <row r="116" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C116" s="7"/>
+    </row>
+    <row r="117" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C117" s="7"/>
+    </row>
+    <row r="118" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C118" s="7"/>
+    </row>
+    <row r="119" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C119" s="7"/>
+    </row>
+    <row r="120" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C120" s="7"/>
+    </row>
+    <row r="121" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C121" s="7"/>
+    </row>
+    <row r="122" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C122" s="7"/>
+    </row>
+    <row r="123" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C123" s="7"/>
+    </row>
+    <row r="124" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C124" s="7"/>
+    </row>
+    <row r="125" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C125" s="7"/>
+    </row>
+    <row r="126" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C126" s="7"/>
+    </row>
+    <row r="127" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="7"/>
+    </row>
+    <row r="128" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C128" s="7"/>
+    </row>
+    <row r="129" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C129" s="7"/>
+    </row>
+    <row r="130" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C130" s="7"/>
+    </row>
+    <row r="131" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C131" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -962,9 +1706,32 @@
     <hyperlink ref="D17" r:id="rId15"/>
     <hyperlink ref="D18" r:id="rId16"/>
     <hyperlink ref="D19" r:id="rId17"/>
+    <hyperlink ref="D21" r:id="rId18"/>
+    <hyperlink ref="D22" r:id="rId19"/>
+    <hyperlink ref="D23" r:id="rId20"/>
+    <hyperlink ref="D24" r:id="rId21"/>
+    <hyperlink ref="D25" r:id="rId22"/>
+    <hyperlink ref="D26" r:id="rId23"/>
+    <hyperlink ref="D28" r:id="rId24"/>
+    <hyperlink ref="D29" r:id="rId25"/>
+    <hyperlink ref="D30" r:id="rId26"/>
+    <hyperlink ref="D31" r:id="rId27"/>
+    <hyperlink ref="D32" r:id="rId28"/>
+    <hyperlink ref="D33" r:id="rId29"/>
+    <hyperlink ref="D34" r:id="rId30"/>
+    <hyperlink ref="D35" r:id="rId31"/>
+    <hyperlink ref="D36" r:id="rId32"/>
+    <hyperlink ref="D37" r:id="rId33"/>
+    <hyperlink ref="D38" r:id="rId34"/>
+    <hyperlink ref="D39" r:id="rId35"/>
+    <hyperlink ref="D40" r:id="rId36"/>
+    <hyperlink ref="D41" r:id="rId37"/>
+    <hyperlink ref="D42" r:id="rId38"/>
+    <hyperlink ref="D43" r:id="rId39"/>
+    <hyperlink ref="D44" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId41"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add Tricks from Lessons 41 to 45
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="138">
   <si>
     <t>Description</t>
   </si>
@@ -425,26 +425,73 @@
     <t>The #id selector styles the element with the specified id.</t>
   </si>
   <si>
-    <t xml:space="preserve">  .selector {
+    <t xml:space="preserve">https://www.w3schools.com/css/css_padding.asp </t>
+  </si>
+  <si>
+    <t>The CSS padding properties are used to generate space around content. The padding clears an area around the content (inside the border) of an element.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/css/css_margin.asp </t>
+  </si>
+  <si>
+    <t>The CSS margin properties are used to generate space around elements. The margin properties set the size of the white space outside the border.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/cssref/pr_padding.asp </t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/css/css_padding.asp</t>
+  </si>
+  <si>
+    <t>The padding shorthand property sets all the padding properties in one declaration. This property can have from one to four values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  selector {
+    margin: 20px 40px 20px 40px;
+  }
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  selector {
+    padding-top: lenght;
+    padding-left: lenght;
+    padding-bottom: lenght;
+    padding-right: lenght;
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> selector {
+    margin-top: lenght;
+    margin-left: lenght;
+    margin-bottom: lenght;
+    margin-right: lenght;
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  selector {
+    padding: 20px 40px 20px 40px;
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  selector {
     padding: value;
   }</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.w3schools.com/css/css_padding.asp </t>
-  </si>
-  <si>
-    <t>The CSS padding properties are used to generate space around content. The padding clears an area around the content (inside the border) of an element.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  .selector {
+    <t xml:space="preserve">  selector {
     margin: value;
   }</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.w3schools.com/css/css_margin.asp </t>
-  </si>
-  <si>
-    <t>The CSS margin properties are used to generate space around elements. The margin properties set the size of the white space outside the border.</t>
+    <t>selector {
+    margin: -length;
+  }</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/cssref/pr_margin.asp</t>
+  </si>
+  <si>
+    <t>The margin shorthand property sets all the margin properties in one declaration. This property can have from one to four values.</t>
   </si>
 </sst>
 </file>
@@ -940,11 +987,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A43" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A49" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="92.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="120.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
     <col min="2" max="2" width="34.375" style="2" bestFit="1" customWidth="1"/>
@@ -953,7 +1000,7 @@
     <col min="5" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
@@ -964,7 +1011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -975,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -986,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -997,7 +1044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1008,7 +1055,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1019,7 +1066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1030,7 +1077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1052,7 +1099,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1063,7 +1110,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
@@ -1074,7 +1121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1085,7 +1132,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1096,7 +1143,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1107,7 +1154,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
@@ -1118,7 +1165,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>57</v>
       </c>
@@ -1129,7 +1176,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
@@ -1140,7 +1187,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
@@ -1151,7 +1198,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>60</v>
       </c>
@@ -1162,7 +1209,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
@@ -1173,7 +1220,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>66</v>
       </c>
@@ -1184,7 +1231,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
@@ -1195,7 +1242,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
@@ -1206,7 +1253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>73</v>
       </c>
@@ -1217,7 +1264,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>83</v>
       </c>
@@ -1228,7 +1275,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
@@ -1239,7 +1286,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>79</v>
       </c>
@@ -1250,7 +1297,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>84</v>
       </c>
@@ -1261,7 +1308,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>89</v>
       </c>
@@ -1272,7 +1319,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>94</v>
       </c>
@@ -1283,7 +1330,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>91</v>
       </c>
@@ -1294,7 +1341,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>97</v>
       </c>
@@ -1305,7 +1352,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>102</v>
       </c>
@@ -1316,7 +1363,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>104</v>
       </c>
@@ -1327,7 +1374,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>101</v>
       </c>
@@ -1338,7 +1385,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>100</v>
       </c>
@@ -1349,7 +1396,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>109</v>
       </c>
@@ -1360,7 +1407,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>112</v>
       </c>
@@ -1371,7 +1418,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>113</v>
       </c>
@@ -1382,7 +1429,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>116</v>
       </c>
@@ -1393,7 +1440,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>119</v>
       </c>
@@ -1404,287 +1451,327 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="7" t="s">
+    </row>
+    <row r="44" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="3" t="s">
+    </row>
+    <row r="45" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
+      <c r="D46" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="D47" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="2:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
     </row>
-    <row r="51" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="7"/>
     </row>
-    <row r="53" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="7"/>
     </row>
-    <row r="54" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="7"/>
     </row>
-    <row r="55" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="7"/>
     </row>
-    <row r="56" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
     </row>
-    <row r="57" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
     </row>
-    <row r="58" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="7"/>
     </row>
-    <row r="59" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="7"/>
     </row>
-    <row r="60" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
     </row>
-    <row r="61" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
     </row>
-    <row r="62" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
     </row>
-    <row r="63" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="7"/>
     </row>
-    <row r="64" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="7"/>
     </row>
-    <row r="65" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
     </row>
-    <row r="66" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
     </row>
-    <row r="67" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="7"/>
     </row>
-    <row r="69" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="7"/>
     </row>
-    <row r="70" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="7"/>
     </row>
-    <row r="71" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
     </row>
-    <row r="72" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="7"/>
     </row>
-    <row r="73" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="7"/>
     </row>
-    <row r="74" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="7"/>
     </row>
-    <row r="75" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
     </row>
-    <row r="76" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
     </row>
-    <row r="77" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
     </row>
-    <row r="78" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="7"/>
     </row>
-    <row r="79" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="7"/>
     </row>
-    <row r="80" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
     </row>
-    <row r="81" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
     </row>
-    <row r="82" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="7"/>
     </row>
-    <row r="83" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
     </row>
-    <row r="84" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="7"/>
     </row>
-    <row r="85" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="7"/>
     </row>
-    <row r="86" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
     </row>
-    <row r="87" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="7"/>
     </row>
-    <row r="88" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="7"/>
     </row>
-    <row r="89" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="7"/>
     </row>
-    <row r="90" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="7"/>
     </row>
-    <row r="91" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
     </row>
-    <row r="92" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="7"/>
     </row>
-    <row r="93" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="7"/>
     </row>
-    <row r="94" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="7"/>
     </row>
-    <row r="95" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
     </row>
-    <row r="96" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="7"/>
     </row>
-    <row r="97" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="7"/>
     </row>
-    <row r="98" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C98" s="7"/>
     </row>
-    <row r="99" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C99" s="7"/>
     </row>
-    <row r="100" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C100" s="7"/>
     </row>
-    <row r="101" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C101" s="7"/>
     </row>
-    <row r="102" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C102" s="7"/>
     </row>
-    <row r="103" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="7"/>
     </row>
-    <row r="104" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C104" s="7"/>
     </row>
-    <row r="105" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C105" s="7"/>
     </row>
-    <row r="106" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C106" s="7"/>
     </row>
-    <row r="107" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C107" s="7"/>
     </row>
-    <row r="108" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C108" s="7"/>
     </row>
-    <row r="109" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C109" s="7"/>
     </row>
-    <row r="110" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C110" s="7"/>
     </row>
-    <row r="111" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C111" s="7"/>
     </row>
-    <row r="112" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C112" s="7"/>
     </row>
-    <row r="113" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C113" s="7"/>
     </row>
-    <row r="114" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C114" s="7"/>
     </row>
-    <row r="115" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C115" s="7"/>
     </row>
-    <row r="116" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="7"/>
     </row>
-    <row r="117" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
     </row>
-    <row r="118" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7"/>
     </row>
-    <row r="119" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C119" s="7"/>
     </row>
-    <row r="120" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C120" s="7"/>
     </row>
-    <row r="121" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C121" s="7"/>
     </row>
-    <row r="122" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C122" s="7"/>
     </row>
-    <row r="123" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C123" s="7"/>
     </row>
-    <row r="124" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C124" s="7"/>
     </row>
-    <row r="125" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C125" s="7"/>
     </row>
-    <row r="126" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C126" s="7"/>
     </row>
-    <row r="127" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C127" s="7"/>
     </row>
-    <row r="128" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="7"/>
     </row>
-    <row r="129" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
     </row>
-    <row r="130" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C130" s="7"/>
     </row>
-    <row r="131" spans="3:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C131" s="7"/>
     </row>
   </sheetData>
@@ -1729,9 +1816,13 @@
     <hyperlink ref="D42" r:id="rId38"/>
     <hyperlink ref="D43" r:id="rId39"/>
     <hyperlink ref="D44" r:id="rId40"/>
+    <hyperlink ref="D45" r:id="rId41"/>
+    <hyperlink ref="D47" r:id="rId42"/>
+    <hyperlink ref="D48" r:id="rId43"/>
+    <hyperlink ref="D49" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId45"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add Tricks from HTML/CSS Lessons 46 to 57
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
   <si>
     <t>Description</t>
   </si>
@@ -492,6 +492,62 @@
   </si>
   <si>
     <t>The margin shorthand property sets all the margin properties in one declaration. This property can have from one to four values.</t>
+  </si>
+  <si>
+    <t>The &lt;body&gt; tag defines the document's body. The &lt;body&gt; element contains all the contents of an HTML document, such as text, hyperlinks, images, tables, lists, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_body.asp </t>
+  </si>
+  <si>
+    <t>&lt;body&gt;</t>
+  </si>
+  <si>
+    <t>CSS Inheritance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/wiki/Inheritance_and_cascade </t>
+  </si>
+  <si>
+    <t>Inheritance in CSS is the mechanism through which certain properties are passed on from a parent element down to its children.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zenorocha.com/css-important/ </t>
+  </si>
+  <si>
+    <t>Class overrides parent style; Second class overrides first class; ID overrides class; Inline overrides ID; !important overrides all</t>
+  </si>
+  <si>
+    <t>CSS Override Style:                                                                                   .pink-text {
+    color: pink !important;
+  }</t>
+  </si>
+  <si>
+    <t>Colors: Hex Code</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/colors/colors_picker.asp</t>
+  </si>
+  <si>
+    <t>Examples: #ff0000, #ccffff, #660066</t>
+  </si>
+  <si>
+    <t>Short Hex Codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.websiteoptimization.com/speed/tweak/hex/ </t>
+  </si>
+  <si>
+    <t>Example: #ff6600 - &gt; #f60</t>
+  </si>
+  <si>
+    <t>Colors: RGB</t>
+  </si>
+  <si>
+    <t>Examples: rgb (255, 0, 0), rgb (218, 112, 214), rgb (160, 82, 45)</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/colors/colors_rgb.asp</t>
   </si>
 </sst>
 </file>
@@ -987,11 +1043,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A49" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A54" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="120.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="93" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
     <col min="2" max="2" width="34.375" style="2" bestFit="1" customWidth="1"/>
@@ -1000,7 +1056,7 @@
     <col min="5" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1011,7 +1067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1022,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1033,7 +1089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1055,7 +1111,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1066,7 +1122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1077,7 +1133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1099,7 +1155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1110,7 +1166,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
@@ -1121,7 +1177,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1132,7 +1188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1143,7 +1199,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1154,7 +1210,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
@@ -1165,7 +1221,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>57</v>
       </c>
@@ -1176,7 +1232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
@@ -1187,7 +1243,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
@@ -1198,7 +1254,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>60</v>
       </c>
@@ -1209,7 +1265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
@@ -1220,7 +1276,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>66</v>
       </c>
@@ -1231,7 +1287,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
@@ -1242,7 +1298,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
@@ -1253,7 +1309,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>73</v>
       </c>
@@ -1264,7 +1320,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>83</v>
       </c>
@@ -1275,7 +1331,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
@@ -1286,7 +1342,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>79</v>
       </c>
@@ -1297,7 +1353,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>84</v>
       </c>
@@ -1308,7 +1364,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>89</v>
       </c>
@@ -1319,7 +1375,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>94</v>
       </c>
@@ -1330,7 +1386,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>91</v>
       </c>
@@ -1341,7 +1397,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>97</v>
       </c>
@@ -1352,7 +1408,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>102</v>
       </c>
@@ -1363,7 +1419,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>104</v>
       </c>
@@ -1374,7 +1430,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>101</v>
       </c>
@@ -1385,7 +1441,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>100</v>
       </c>
@@ -1396,7 +1452,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>109</v>
       </c>
@@ -1407,7 +1463,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>112</v>
       </c>
@@ -1418,7 +1474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>113</v>
       </c>
@@ -1429,7 +1485,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>116</v>
       </c>
@@ -1440,7 +1496,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>119</v>
       </c>
@@ -1451,7 +1507,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>133</v>
       </c>
@@ -1462,7 +1518,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>134</v>
       </c>
@@ -1473,7 +1529,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>135</v>
       </c>
@@ -1484,7 +1540,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>130</v>
       </c>
@@ -1495,7 +1551,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>131</v>
       </c>
@@ -1506,7 +1562,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>132</v>
       </c>
@@ -1517,7 +1573,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>129</v>
       </c>
@@ -1528,250 +1584,298 @@
         <v>136</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="7"/>
-    </row>
-    <row r="51" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="7"/>
-    </row>
-    <row r="52" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="7"/>
-    </row>
-    <row r="53" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="7"/>
-    </row>
-    <row r="55" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="7"/>
-    </row>
-    <row r="56" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
     </row>
-    <row r="57" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
     </row>
-    <row r="58" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="7"/>
     </row>
-    <row r="59" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="7"/>
     </row>
-    <row r="60" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
     </row>
-    <row r="61" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
     </row>
-    <row r="62" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
     </row>
-    <row r="63" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="7"/>
     </row>
-    <row r="64" spans="2:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="7"/>
     </row>
-    <row r="65" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
     </row>
-    <row r="66" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
     </row>
-    <row r="67" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="7"/>
     </row>
-    <row r="69" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="7"/>
     </row>
-    <row r="70" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="7"/>
     </row>
-    <row r="71" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
     </row>
-    <row r="72" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="7"/>
     </row>
-    <row r="73" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="7"/>
     </row>
-    <row r="74" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="7"/>
     </row>
-    <row r="75" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
     </row>
-    <row r="76" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
     </row>
-    <row r="77" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
     </row>
-    <row r="78" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="7"/>
     </row>
-    <row r="79" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="7"/>
     </row>
-    <row r="80" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
     </row>
-    <row r="81" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
     </row>
-    <row r="82" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="7"/>
     </row>
-    <row r="83" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
     </row>
-    <row r="84" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="7"/>
     </row>
-    <row r="85" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="7"/>
     </row>
-    <row r="86" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
     </row>
-    <row r="87" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="7"/>
     </row>
-    <row r="88" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="7"/>
     </row>
-    <row r="89" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="7"/>
     </row>
-    <row r="90" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="7"/>
     </row>
-    <row r="91" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
     </row>
-    <row r="92" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="7"/>
     </row>
-    <row r="93" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="7"/>
     </row>
-    <row r="94" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="7"/>
     </row>
-    <row r="95" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
     </row>
-    <row r="96" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="7"/>
     </row>
-    <row r="97" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="7"/>
     </row>
-    <row r="98" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C98" s="7"/>
     </row>
-    <row r="99" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C99" s="7"/>
     </row>
-    <row r="100" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C100" s="7"/>
     </row>
-    <row r="101" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C101" s="7"/>
     </row>
-    <row r="102" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C102" s="7"/>
     </row>
-    <row r="103" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="7"/>
     </row>
-    <row r="104" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C104" s="7"/>
     </row>
-    <row r="105" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C105" s="7"/>
     </row>
-    <row r="106" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C106" s="7"/>
     </row>
-    <row r="107" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C107" s="7"/>
     </row>
-    <row r="108" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C108" s="7"/>
     </row>
-    <row r="109" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C109" s="7"/>
     </row>
-    <row r="110" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C110" s="7"/>
     </row>
-    <row r="111" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C111" s="7"/>
     </row>
-    <row r="112" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C112" s="7"/>
     </row>
-    <row r="113" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C113" s="7"/>
     </row>
-    <row r="114" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C114" s="7"/>
     </row>
-    <row r="115" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C115" s="7"/>
     </row>
-    <row r="116" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="7"/>
     </row>
-    <row r="117" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
     </row>
-    <row r="118" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7"/>
     </row>
-    <row r="119" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C119" s="7"/>
     </row>
-    <row r="120" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C120" s="7"/>
     </row>
-    <row r="121" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C121" s="7"/>
     </row>
-    <row r="122" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C122" s="7"/>
     </row>
-    <row r="123" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C123" s="7"/>
     </row>
-    <row r="124" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C124" s="7"/>
     </row>
-    <row r="125" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C125" s="7"/>
     </row>
-    <row r="126" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C126" s="7"/>
     </row>
-    <row r="127" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C127" s="7"/>
     </row>
-    <row r="128" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="7"/>
     </row>
-    <row r="129" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
     </row>
-    <row r="130" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C130" s="7"/>
     </row>
-    <row r="131" spans="3:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C131" s="7"/>
     </row>
   </sheetData>
@@ -1820,9 +1924,15 @@
     <hyperlink ref="D47" r:id="rId42"/>
     <hyperlink ref="D48" r:id="rId43"/>
     <hyperlink ref="D49" r:id="rId44"/>
+    <hyperlink ref="D50" r:id="rId45"/>
+    <hyperlink ref="D51" r:id="rId46"/>
+    <hyperlink ref="D52" r:id="rId47"/>
+    <hyperlink ref="D53" r:id="rId48"/>
+    <hyperlink ref="D54" r:id="rId49"/>
+    <hyperlink ref="D55" r:id="rId50"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId45"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId51"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add Tricks from Bootstrap Lessons 01 to 05
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="6" r:id="rId1"/>
     <sheet name="HTML-CSS" sheetId="1" r:id="rId2"/>
-    <sheet name="Bootstrap" sheetId="3" r:id="rId3"/>
+    <sheet name="Bootstrap 3" sheetId="3" r:id="rId3"/>
     <sheet name="Font Awesome" sheetId="4" r:id="rId4"/>
     <sheet name="Animated" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="177">
   <si>
     <t>Description</t>
   </si>
@@ -548,6 +548,70 @@
   </si>
   <si>
     <t>https://www.w3schools.com/colors/colors_rgb.asp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://getbootstrap.com/css/#overview-container </t>
+  </si>
+  <si>
+    <t>Bootstrap requires a containing element to wrap site contents and house our grid system. Use .container-fluid for a full width container, spanning the entire width of your viewport.</t>
+  </si>
+  <si>
+    <t>&lt;div class="container-fluid"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="container"&gt;</t>
+  </si>
+  <si>
+    <t>Bootstrap requires a containing element to wrap site contents and house our grid system. Use .container for a responsive fixed width container.</t>
+  </si>
+  <si>
+    <t>Images in Bootstrap 3 can be made responsive-friendly via the addition of the .img-responsive class. This applies max-width: 100%;, height: auto; and display: block; to the image so that it scales nicely to the parent element.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://getbootstrap.com/css/#images </t>
+  </si>
+  <si>
+    <t>&lt;img class="img-responsive"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img class="img-responsive center-block"&gt;</t>
+  </si>
+  <si>
+    <t>To center images which use the .img-responsive class, use .center-block instead of .text-center.</t>
+  </si>
+  <si>
+    <t>&lt;element class="center-block"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set an element to display: block and center via margin. Available as a mixin and class.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://getbootstrap.com/css/#helper-classes </t>
+  </si>
+  <si>
+    <t>&lt;element class="text-center&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://getbootstrap.com/css/#type-alignment </t>
+  </si>
+  <si>
+    <t>Center aligned text</t>
+  </si>
+  <si>
+    <t>&lt;button class="btn"&gt;</t>
+  </si>
+  <si>
+    <t>http://getbootstrap.com/css/?#buttons-tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/bootstrap/bootstrap_buttons.asp </t>
+  </si>
+  <si>
+    <t>&lt;button class="btn btn-block"&gt;</t>
+  </si>
+  <si>
+    <t>Add class .btn-block to create a block level button</t>
   </si>
 </sst>
 </file>
@@ -632,7 +696,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,6 +717,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1043,9 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A54" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
-    </sheetView>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="93" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1943,12 +2011,129 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E10"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="22" defaultRowHeight="108" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="22" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" location="overview-container "/>
+    <hyperlink ref="D4" r:id="rId2" location="overview-container "/>
+    <hyperlink ref="D5" r:id="rId3" location="images "/>
+    <hyperlink ref="D6" r:id="rId4" location="images "/>
+    <hyperlink ref="D7" r:id="rId5" location="helper-classes "/>
+    <hyperlink ref="D8" r:id="rId6" location="type-alignment "/>
+    <hyperlink ref="D9" r:id="rId7" location="buttons-tags"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Add Tricks from Bootstrap Lessons 06 to 08
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Font Awesome" sheetId="4" r:id="rId4"/>
     <sheet name="Animated" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="181">
   <si>
     <t>Description</t>
   </si>
@@ -612,6 +612,18 @@
   </si>
   <si>
     <t>Add class .btn-block to create a block level button</t>
+  </si>
+  <si>
+    <t>Basic Button</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/bootstrap/bootstrap_buttons.asp</t>
+  </si>
+  <si>
+    <t>&lt;button class="btn-primary"&gt;; &lt;button class="btn-info"&gt;; &lt;button class="btn-danger"&gt;;</t>
+  </si>
+  <si>
+    <t>Button Styles</t>
   </si>
 </sst>
 </file>
@@ -2011,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E10"/>
+  <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="108" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2108,6 +2120,9 @@
       <c r="B9" s="2" t="s">
         <v>172</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="D9" s="9" t="s">
         <v>173</v>
       </c>
@@ -2121,6 +2136,20 @@
       </c>
       <c r="C10" s="5" t="s">
         <v>176</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2133,6 +2162,8 @@
     <hyperlink ref="D8" r:id="rId6" location="type-alignment "/>
     <hyperlink ref="D9" r:id="rId7" location="buttons-tags"/>
     <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Add Tricks from Lessons 09 to 10
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="187">
   <si>
     <t>Description</t>
   </si>
@@ -624,6 +624,27 @@
   </si>
   <si>
     <t>Button Styles</t>
+  </si>
+  <si>
+    <t>&lt;div class="container"&gt;
+  &lt;div class="row"&gt;
+    &lt;div class="col-*-*"&gt;&lt;/div&gt;
+  &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Bootstrap's grid system allows up to 12 columns across the page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/bootstrap/bootstrap_grid_system.asp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/bootstrap/bootstrap_ref_css_helpers.asp </t>
+  </si>
+  <si>
+    <t>&lt;element class="text-primary"&gt;; &lt;element class="text-danger"&gt;; &lt;element class="text-info"&gt;;</t>
+  </si>
+  <si>
+    <t>Add meaning through text-colors.</t>
   </si>
 </sst>
 </file>
@@ -2023,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="108" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2152,6 +2173,28 @@
         <v>178</v>
       </c>
     </row>
+    <row r="12" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="overview-container "/>
@@ -2164,6 +2207,8 @@
     <hyperlink ref="E9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Add Tricks from Bootstrap lessons 11 to 12
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="190">
   <si>
     <t>Description</t>
   </si>
@@ -646,12 +646,21 @@
   <si>
     <t>Add meaning through text-colors.</t>
   </si>
+  <si>
+    <t>The &lt;span&gt; tag is used to group inline-elements in a document. The &lt;span&gt; tag provides no visual change by itself. The &lt;span&gt; tag provides a way to add a hook to a part of a text or a part of a document.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lorem ipsum dolor sit amet,&lt;span id="span-id"&gt;consectetur&lt;/span&gt;&lt;p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_span.asp </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -699,6 +708,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -729,7 +746,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,6 +774,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2044,10 +2064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E13"/>
+  <dimension ref="B1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="108" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2195,6 +2215,20 @@
         <v>184</v>
       </c>
     </row>
+    <row r="14" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="overview-container "/>
@@ -2209,8 +2243,10 @@
     <hyperlink ref="D11" r:id="rId10"/>
     <hyperlink ref="D12" r:id="rId11"/>
     <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId14"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2221,12 +2257,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="24.125" defaultRowHeight="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2240,7 +2294,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Tags header main footer session att for novalidate
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="204">
   <si>
     <t>Description</t>
   </si>
@@ -388,9 +388,6 @@
     <t xml:space="preserve">https://www.w3schools.com/tags/tag_div.asp </t>
   </si>
   <si>
-    <t>The &lt;div&gt; tag defines a division or a section in an HTML document. The &lt;div&gt; tag is used to group block-elements to format them with CSS.</t>
-  </si>
-  <si>
     <t>&lt;div class="class-name"&gt;</t>
   </si>
   <si>
@@ -662,7 +659,44 @@
     <t xml:space="preserve">https://www.w3schools.com/tags/tag_header.asp </t>
   </si>
   <si>
-    <t>The &lt;header&gt; element represents a container for introductory content or a set of navigational links.</t>
+    <t xml:space="preserve">https://www.w3schools.com/tags/tag_main.asp </t>
+  </si>
+  <si>
+    <t>&lt;main&gt;</t>
+  </si>
+  <si>
+    <t>&lt;footer&gt;</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/tag_footer.asp</t>
+  </si>
+  <si>
+    <t>The &lt;footer&gt; tag defines a footer for a document or section. A &lt;footer&gt; element should contain information about its containing element. A &lt;footer&gt; element typically contains: authorship information, copyright information, contact information, sitemap, back to top links, related documents. You can have several &lt;footer&gt; elements in one document.</t>
+  </si>
+  <si>
+    <t>The &lt;main&gt; tag specifies the main content of a document. The content inside the &lt;main&gt; element should be unique to the document. It should not contain any content that is repeated across documents such as sidebars, navigation links, copyright information, site logos, and search forms. Note: There must not be more than one &lt;main&gt; element in a document. The &lt;main&gt; element must NOT be a descendant of an &lt;article&gt;, &lt;aside&gt;, &lt;footer&gt;, &lt;header&gt;, or &lt;nav&gt; element.</t>
+  </si>
+  <si>
+    <t>The &lt;div&gt; tag defines a division or a section in an HTML document. The &lt;div&gt; tag is used to group block-elements to format them with CSS. &lt;div&gt; position is always "above" and "left" its next elements.</t>
+  </si>
+  <si>
+    <t>&lt;form action="/submit-cat-photo" novalidate&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The novalidate attribute is a boolean attribute. When present, it specifies that the form-data (input) should not be validated when submitted.
+</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/att_form_novalidate.asp</t>
+  </si>
+  <si>
+    <t>&lt;label for="string"&gt;</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/att_label_for.asp</t>
+  </si>
+  <si>
+    <t>The for attribute specifies which form element a label is bound to.</t>
   </si>
 </sst>
 </file>
@@ -1173,22 +1207,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D131"/>
+  <dimension ref="B2:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A55" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B39" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="93" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="155.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="34.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71.375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1199,7 +1233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +1255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1232,7 +1266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1243,7 +1277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1254,7 +1288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1299,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1276,7 +1310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1287,7 +1321,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1298,7 +1332,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
@@ -1309,7 +1343,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1320,7 +1354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1331,7 +1365,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1342,7 +1376,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
@@ -1353,7 +1387,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>57</v>
       </c>
@@ -1364,7 +1398,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
@@ -1375,7 +1409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
@@ -1386,7 +1420,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>60</v>
       </c>
@@ -1397,7 +1431,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
@@ -1408,7 +1442,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>66</v>
       </c>
@@ -1419,7 +1453,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
@@ -1430,7 +1464,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
@@ -1441,7 +1475,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>73</v>
       </c>
@@ -1452,7 +1486,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>83</v>
       </c>
@@ -1463,7 +1497,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
@@ -1474,7 +1508,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>79</v>
       </c>
@@ -1485,7 +1519,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>84</v>
       </c>
@@ -1496,7 +1530,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>89</v>
       </c>
@@ -1507,53 +1541,53 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+    <row r="33" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+    <row r="34" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
+    <row r="35" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>86</v>
@@ -1562,461 +1596,499 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+    <row r="36" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+    <row r="38" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+    <row r="39" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C40" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
+      <c r="C41" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+      <c r="C42" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C40" s="7" t="s">
+    </row>
+    <row r="43" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+      <c r="C43" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="3" t="s">
+    </row>
+    <row r="44" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+      <c r="C44" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="7" t="s">
+    </row>
+    <row r="45" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
+    </row>
+    <row r="46" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C46" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="3" t="s">
+    </row>
+    <row r="47" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="D52" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
+      <c r="C53" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C51" s="7" t="s">
+    </row>
+    <row r="54" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
+    </row>
+    <row r="55" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
+      <c r="C55" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C53" s="7" t="s">
+    </row>
+    <row r="56" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
+      <c r="C56" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C54" s="7" t="s">
+    </row>
+    <row r="57" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
+      <c r="C57" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="D57" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
+    </row>
+    <row r="58" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C56" s="7" t="s">
+    </row>
+    <row r="59" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="C59" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="7"/>
-    </row>
-    <row r="58" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="7"/>
-    </row>
-    <row r="59" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="7"/>
-    </row>
-    <row r="61" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
     </row>
-    <row r="62" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
     </row>
-    <row r="63" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="7"/>
     </row>
-    <row r="64" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="7"/>
     </row>
-    <row r="65" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
     </row>
-    <row r="66" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
     </row>
-    <row r="67" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="7"/>
     </row>
-    <row r="69" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="7"/>
     </row>
-    <row r="70" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="7"/>
     </row>
-    <row r="71" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
     </row>
-    <row r="72" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="7"/>
     </row>
-    <row r="73" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="7"/>
     </row>
-    <row r="74" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="7"/>
     </row>
-    <row r="75" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
     </row>
-    <row r="76" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
     </row>
-    <row r="77" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
     </row>
-    <row r="78" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="7"/>
     </row>
-    <row r="79" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="7"/>
     </row>
-    <row r="80" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
     </row>
-    <row r="81" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
     </row>
-    <row r="82" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="7"/>
     </row>
-    <row r="83" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
     </row>
-    <row r="84" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="7"/>
     </row>
-    <row r="85" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="7"/>
     </row>
-    <row r="86" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
     </row>
-    <row r="87" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="7"/>
     </row>
-    <row r="88" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="7"/>
     </row>
-    <row r="89" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="7"/>
     </row>
-    <row r="90" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="7"/>
     </row>
-    <row r="91" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
     </row>
-    <row r="92" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="7"/>
     </row>
-    <row r="93" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="7"/>
     </row>
-    <row r="94" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="7"/>
     </row>
-    <row r="95" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
     </row>
-    <row r="96" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="7"/>
     </row>
-    <row r="97" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="7"/>
     </row>
-    <row r="98" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C98" s="7"/>
     </row>
-    <row r="99" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C99" s="7"/>
     </row>
-    <row r="100" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C100" s="7"/>
     </row>
-    <row r="101" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C101" s="7"/>
     </row>
-    <row r="102" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C102" s="7"/>
     </row>
-    <row r="103" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="7"/>
     </row>
-    <row r="104" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C104" s="7"/>
     </row>
-    <row r="105" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C105" s="7"/>
     </row>
-    <row r="106" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C106" s="7"/>
     </row>
-    <row r="107" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C107" s="7"/>
     </row>
-    <row r="108" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C108" s="7"/>
     </row>
-    <row r="109" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C109" s="7"/>
     </row>
-    <row r="110" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C110" s="7"/>
     </row>
-    <row r="111" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C111" s="7"/>
     </row>
-    <row r="112" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C112" s="7"/>
     </row>
-    <row r="113" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C113" s="7"/>
     </row>
-    <row r="114" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C114" s="7"/>
     </row>
-    <row r="115" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C115" s="7"/>
     </row>
-    <row r="116" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="7"/>
     </row>
-    <row r="117" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
     </row>
-    <row r="118" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7"/>
     </row>
-    <row r="119" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C119" s="7"/>
     </row>
-    <row r="120" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C120" s="7"/>
     </row>
-    <row r="121" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C121" s="7"/>
     </row>
-    <row r="122" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C122" s="7"/>
     </row>
-    <row r="123" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C123" s="7"/>
     </row>
-    <row r="124" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C124" s="7"/>
     </row>
-    <row r="125" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C125" s="7"/>
     </row>
-    <row r="126" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C126" s="7"/>
     </row>
-    <row r="127" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C127" s="7"/>
     </row>
-    <row r="128" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="7"/>
     </row>
-    <row r="129" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
     </row>
-    <row r="130" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C130" s="7"/>
     </row>
-    <row r="131" spans="3:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C131" s="7"/>
+    </row>
+    <row r="132" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C132" s="7"/>
+    </row>
+    <row r="133" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C133" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2046,34 +2118,38 @@
     <hyperlink ref="D28" r:id="rId24"/>
     <hyperlink ref="D29" r:id="rId25"/>
     <hyperlink ref="D30" r:id="rId26"/>
-    <hyperlink ref="D31" r:id="rId27"/>
-    <hyperlink ref="D32" r:id="rId28"/>
-    <hyperlink ref="D33" r:id="rId29"/>
-    <hyperlink ref="D34" r:id="rId30"/>
-    <hyperlink ref="D35" r:id="rId31"/>
-    <hyperlink ref="D36" r:id="rId32"/>
-    <hyperlink ref="D37" r:id="rId33"/>
-    <hyperlink ref="D38" r:id="rId34"/>
-    <hyperlink ref="D39" r:id="rId35"/>
-    <hyperlink ref="D40" r:id="rId36"/>
-    <hyperlink ref="D41" r:id="rId37"/>
-    <hyperlink ref="D42" r:id="rId38"/>
-    <hyperlink ref="D43" r:id="rId39"/>
-    <hyperlink ref="D44" r:id="rId40"/>
-    <hyperlink ref="D45" r:id="rId41"/>
-    <hyperlink ref="D47" r:id="rId42"/>
-    <hyperlink ref="D48" r:id="rId43"/>
-    <hyperlink ref="D49" r:id="rId44"/>
-    <hyperlink ref="D50" r:id="rId45"/>
-    <hyperlink ref="D51" r:id="rId46"/>
-    <hyperlink ref="D52" r:id="rId47"/>
-    <hyperlink ref="D53" r:id="rId48"/>
-    <hyperlink ref="D54" r:id="rId49"/>
-    <hyperlink ref="D55" r:id="rId50"/>
-    <hyperlink ref="D56" r:id="rId51"/>
+    <hyperlink ref="D32" r:id="rId27"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D35" r:id="rId30"/>
+    <hyperlink ref="D36" r:id="rId31"/>
+    <hyperlink ref="D37" r:id="rId32"/>
+    <hyperlink ref="D38" r:id="rId33"/>
+    <hyperlink ref="D40" r:id="rId34"/>
+    <hyperlink ref="D41" r:id="rId35"/>
+    <hyperlink ref="D42" r:id="rId36"/>
+    <hyperlink ref="D43" r:id="rId37"/>
+    <hyperlink ref="D44" r:id="rId38"/>
+    <hyperlink ref="D45" r:id="rId39"/>
+    <hyperlink ref="D46" r:id="rId40"/>
+    <hyperlink ref="D47" r:id="rId41"/>
+    <hyperlink ref="D49" r:id="rId42"/>
+    <hyperlink ref="D50" r:id="rId43"/>
+    <hyperlink ref="D51" r:id="rId44"/>
+    <hyperlink ref="D52" r:id="rId45"/>
+    <hyperlink ref="D53" r:id="rId46"/>
+    <hyperlink ref="D54" r:id="rId47"/>
+    <hyperlink ref="D55" r:id="rId48"/>
+    <hyperlink ref="D56" r:id="rId49"/>
+    <hyperlink ref="D57" r:id="rId50"/>
+    <hyperlink ref="D58" r:id="rId51"/>
+    <hyperlink ref="D59" r:id="rId52"/>
+    <hyperlink ref="D60" r:id="rId53"/>
+    <hyperlink ref="D31" r:id="rId54"/>
+    <hyperlink ref="D39" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId52"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId56"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2113,137 +2189,137 @@
     </row>
     <row r="3" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="D10" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="D11" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="D13" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Some new tricks - header of main and sections done
</commit_message>
<xml_diff>
--- a/Front End Tricks/Front End Tricks.xlsx
+++ b/Front End Tricks/Front End Tricks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="207">
   <si>
     <t>Description</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Placeholder Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://br.lipsum.com/ </t>
   </si>
   <si>
     <t>Change color; Inline CSS</t>
@@ -187,9 +184,6 @@
     <t xml:space="preserve">https://www.w3schools.com/tags/tag_img.asp </t>
   </si>
   <si>
-    <t>&lt;img src="URL" alt="alternate text&gt;</t>
-  </si>
-  <si>
     <t>The &lt;img&gt; tag defines an image in an HTML page.</t>
   </si>
   <si>
@@ -697,6 +691,21 @@
   </si>
   <si>
     <t>The for attribute specifies which form element a label is bound to.</t>
+  </si>
+  <si>
+    <t>http://www.blindtextgenerator.com/lorem-ipsum</t>
+  </si>
+  <si>
+    <t>&lt;img src="URL" title="title"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="URL" alt="alternate text"&gt;</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/att_title.asp</t>
+  </si>
+  <si>
+    <t>The title attribute specifies extra information about an element. The information is most often shown as a tooltip text when the mouse moves over the element.</t>
   </si>
 </sst>
 </file>
@@ -1182,22 +1191,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1207,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D133"/>
+  <dimension ref="B2:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B39" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="155.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1274,605 +1283,613 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>46</v>
+      <c r="B16" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>48</v>
+        <v>206</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>56</v>
+      <c r="B18" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="4" t="s">
+    </row>
+    <row r="23" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="28" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>198</v>
+        <v>87</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>200</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>93</v>
+        <v>197</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>92</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>97</v>
+      <c r="B34" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>197</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>110</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C42" s="7" t="s">
+    </row>
+    <row r="44" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
+      <c r="D44" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>139</v>
+      <c r="B52" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>151</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="7"/>
+      <c r="D61" s="3" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="62" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
@@ -2089,6 +2106,9 @@
     </row>
     <row r="133" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C133" s="7"/>
+    </row>
+    <row r="134" spans="3:3" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C134" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2105,51 +2125,52 @@
     <hyperlink ref="D13" r:id="rId11"/>
     <hyperlink ref="D14" r:id="rId12"/>
     <hyperlink ref="D15" r:id="rId13"/>
-    <hyperlink ref="D16" r:id="rId14"/>
-    <hyperlink ref="D17" r:id="rId15"/>
-    <hyperlink ref="D18" r:id="rId16"/>
-    <hyperlink ref="D19" r:id="rId17"/>
-    <hyperlink ref="D21" r:id="rId18"/>
-    <hyperlink ref="D22" r:id="rId19"/>
-    <hyperlink ref="D23" r:id="rId20"/>
-    <hyperlink ref="D24" r:id="rId21"/>
-    <hyperlink ref="D25" r:id="rId22"/>
-    <hyperlink ref="D26" r:id="rId23"/>
-    <hyperlink ref="D28" r:id="rId24"/>
-    <hyperlink ref="D29" r:id="rId25"/>
-    <hyperlink ref="D30" r:id="rId26"/>
-    <hyperlink ref="D32" r:id="rId27"/>
-    <hyperlink ref="D33" r:id="rId28"/>
-    <hyperlink ref="D34" r:id="rId29"/>
-    <hyperlink ref="D35" r:id="rId30"/>
-    <hyperlink ref="D36" r:id="rId31"/>
-    <hyperlink ref="D37" r:id="rId32"/>
-    <hyperlink ref="D38" r:id="rId33"/>
-    <hyperlink ref="D40" r:id="rId34"/>
-    <hyperlink ref="D41" r:id="rId35"/>
-    <hyperlink ref="D42" r:id="rId36"/>
-    <hyperlink ref="D43" r:id="rId37"/>
-    <hyperlink ref="D44" r:id="rId38"/>
-    <hyperlink ref="D45" r:id="rId39"/>
-    <hyperlink ref="D46" r:id="rId40"/>
-    <hyperlink ref="D47" r:id="rId41"/>
-    <hyperlink ref="D49" r:id="rId42"/>
-    <hyperlink ref="D50" r:id="rId43"/>
-    <hyperlink ref="D51" r:id="rId44"/>
-    <hyperlink ref="D52" r:id="rId45"/>
-    <hyperlink ref="D53" r:id="rId46"/>
-    <hyperlink ref="D54" r:id="rId47"/>
-    <hyperlink ref="D55" r:id="rId48"/>
-    <hyperlink ref="D56" r:id="rId49"/>
-    <hyperlink ref="D57" r:id="rId50"/>
-    <hyperlink ref="D58" r:id="rId51"/>
-    <hyperlink ref="D59" r:id="rId52"/>
-    <hyperlink ref="D60" r:id="rId53"/>
-    <hyperlink ref="D31" r:id="rId54"/>
-    <hyperlink ref="D39" r:id="rId55"/>
+    <hyperlink ref="D17" r:id="rId14"/>
+    <hyperlink ref="D18" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D22" r:id="rId18"/>
+    <hyperlink ref="D23" r:id="rId19"/>
+    <hyperlink ref="D24" r:id="rId20"/>
+    <hyperlink ref="D25" r:id="rId21"/>
+    <hyperlink ref="D26" r:id="rId22"/>
+    <hyperlink ref="D27" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D33" r:id="rId27"/>
+    <hyperlink ref="D34" r:id="rId28"/>
+    <hyperlink ref="D35" r:id="rId29"/>
+    <hyperlink ref="D36" r:id="rId30"/>
+    <hyperlink ref="D37" r:id="rId31"/>
+    <hyperlink ref="D38" r:id="rId32"/>
+    <hyperlink ref="D39" r:id="rId33"/>
+    <hyperlink ref="D41" r:id="rId34"/>
+    <hyperlink ref="D42" r:id="rId35"/>
+    <hyperlink ref="D43" r:id="rId36"/>
+    <hyperlink ref="D44" r:id="rId37"/>
+    <hyperlink ref="D45" r:id="rId38"/>
+    <hyperlink ref="D46" r:id="rId39"/>
+    <hyperlink ref="D47" r:id="rId40"/>
+    <hyperlink ref="D48" r:id="rId41"/>
+    <hyperlink ref="D50" r:id="rId42"/>
+    <hyperlink ref="D51" r:id="rId43"/>
+    <hyperlink ref="D52" r:id="rId44"/>
+    <hyperlink ref="D53" r:id="rId45"/>
+    <hyperlink ref="D54" r:id="rId46"/>
+    <hyperlink ref="D55" r:id="rId47"/>
+    <hyperlink ref="D56" r:id="rId48"/>
+    <hyperlink ref="D57" r:id="rId49"/>
+    <hyperlink ref="D58" r:id="rId50"/>
+    <hyperlink ref="D59" r:id="rId51"/>
+    <hyperlink ref="D60" r:id="rId52"/>
+    <hyperlink ref="D61" r:id="rId53"/>
+    <hyperlink ref="D32" r:id="rId54"/>
+    <hyperlink ref="D40" r:id="rId55"/>
+    <hyperlink ref="D16" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId57"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2163,7 +2184,7 @@
   <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="108" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2189,137 +2210,137 @@
     </row>
     <row r="3" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>